<commit_message>
Atualizado por script em 20-12-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/germany_bundesliga_2023-2024.xlsx
+++ b/2023/germany_bundesliga_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V135"/>
+  <dimension ref="A1:V138"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6461,22 +6461,22 @@
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>Bayer Leverkusen</t>
+          <t>Stuttgart</t>
         </is>
       </c>
       <c r="I66" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J66" t="n">
-        <v>2.83</v>
+        <v>2.3</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
@@ -6484,15 +6484,15 @@
         </is>
       </c>
       <c r="L66" t="n">
-        <v>4.47</v>
+        <v>2.61</v>
       </c>
       <c r="M66" t="inlineStr">
         <is>
-          <t>21/10/2023 15:00</t>
+          <t>21/10/2023 15:29</t>
         </is>
       </c>
       <c r="N66" t="n">
-        <v>3.69</v>
+        <v>3.46</v>
       </c>
       <c r="O66" t="inlineStr">
         <is>
@@ -6500,15 +6500,15 @@
         </is>
       </c>
       <c r="P66" t="n">
-        <v>4.11</v>
+        <v>3.37</v>
       </c>
       <c r="Q66" t="inlineStr">
         <is>
-          <t>21/10/2023 14:58</t>
+          <t>21/10/2023 15:28</t>
         </is>
       </c>
       <c r="R66" t="n">
-        <v>2.52</v>
+        <v>3.34</v>
       </c>
       <c r="S66" t="inlineStr">
         <is>
@@ -6516,16 +6516,16 @@
         </is>
       </c>
       <c r="T66" t="n">
-        <v>1.79</v>
+        <v>2.92</v>
       </c>
       <c r="U66" t="inlineStr">
         <is>
-          <t>21/10/2023 15:00</t>
+          <t>21/10/2023 15:29</t>
         </is>
       </c>
       <c r="V66" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/wolfsburg-bayer-leverkusen/xdGA36uU/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/union-berlin-vfb-stuttgart/plb35SAH/</t>
         </is>
       </c>
     </row>
@@ -6553,22 +6553,22 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Hoffenheim</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>Stuttgart</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="I67" t="n">
         <v>3</v>
       </c>
       <c r="J67" t="n">
-        <v>2.3</v>
+        <v>2.39</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
@@ -6576,15 +6576,15 @@
         </is>
       </c>
       <c r="L67" t="n">
-        <v>2.61</v>
+        <v>2.06</v>
       </c>
       <c r="M67" t="inlineStr">
         <is>
-          <t>21/10/2023 15:29</t>
+          <t>21/10/2023 15:28</t>
         </is>
       </c>
       <c r="N67" t="n">
-        <v>3.46</v>
+        <v>3.56</v>
       </c>
       <c r="O67" t="inlineStr">
         <is>
@@ -6592,32 +6592,32 @@
         </is>
       </c>
       <c r="P67" t="n">
-        <v>3.37</v>
+        <v>3.65</v>
       </c>
       <c r="Q67" t="inlineStr">
         <is>
+          <t>21/10/2023 15:26</t>
+        </is>
+      </c>
+      <c r="R67" t="n">
+        <v>2.98</v>
+      </c>
+      <c r="S67" t="inlineStr">
+        <is>
+          <t>01/10/2023 23:01</t>
+        </is>
+      </c>
+      <c r="T67" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="U67" t="inlineStr">
+        <is>
           <t>21/10/2023 15:28</t>
         </is>
       </c>
-      <c r="R67" t="n">
-        <v>3.34</v>
-      </c>
-      <c r="S67" t="inlineStr">
-        <is>
-          <t>01/10/2023 23:01</t>
-        </is>
-      </c>
-      <c r="T67" t="n">
-        <v>2.92</v>
-      </c>
-      <c r="U67" t="inlineStr">
-        <is>
-          <t>21/10/2023 15:29</t>
-        </is>
-      </c>
       <c r="V67" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/union-berlin-vfb-stuttgart/plb35SAH/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/hoffenheim-eintracht-frankfurt/fDpPMTuh/</t>
         </is>
       </c>
     </row>
@@ -6645,7 +6645,7 @@
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Hoffenheim</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="G68" t="n">
@@ -6653,14 +6653,14 @@
       </c>
       <c r="H68" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Bayer Leverkusen</t>
         </is>
       </c>
       <c r="I68" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J68" t="n">
-        <v>2.39</v>
+        <v>2.83</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
@@ -6668,15 +6668,15 @@
         </is>
       </c>
       <c r="L68" t="n">
-        <v>2.06</v>
+        <v>4.47</v>
       </c>
       <c r="M68" t="inlineStr">
         <is>
-          <t>21/10/2023 15:28</t>
+          <t>21/10/2023 15:00</t>
         </is>
       </c>
       <c r="N68" t="n">
-        <v>3.56</v>
+        <v>3.69</v>
       </c>
       <c r="O68" t="inlineStr">
         <is>
@@ -6684,15 +6684,15 @@
         </is>
       </c>
       <c r="P68" t="n">
-        <v>3.65</v>
+        <v>4.11</v>
       </c>
       <c r="Q68" t="inlineStr">
         <is>
-          <t>21/10/2023 15:26</t>
+          <t>21/10/2023 14:58</t>
         </is>
       </c>
       <c r="R68" t="n">
-        <v>2.98</v>
+        <v>2.52</v>
       </c>
       <c r="S68" t="inlineStr">
         <is>
@@ -6700,16 +6700,16 @@
         </is>
       </c>
       <c r="T68" t="n">
-        <v>3.79</v>
+        <v>1.79</v>
       </c>
       <c r="U68" t="inlineStr">
         <is>
-          <t>21/10/2023 15:28</t>
+          <t>21/10/2023 15:00</t>
         </is>
       </c>
       <c r="V68" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/hoffenheim-eintracht-frankfurt/fDpPMTuh/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/wolfsburg-bayer-leverkusen/xdGA36uU/</t>
         </is>
       </c>
     </row>
@@ -6737,71 +6737,71 @@
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Darmstadt</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H69" t="inlineStr">
         <is>
-          <t>Bochum</t>
+          <t>RB Leipzig</t>
         </is>
       </c>
       <c r="I69" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J69" t="n">
-        <v>1.56</v>
+        <v>6.5</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>01/10/2023 23:02</t>
+          <t>02/10/2023 08:32</t>
         </is>
       </c>
       <c r="L69" t="n">
-        <v>1.81</v>
+        <v>6.59</v>
       </c>
       <c r="M69" t="inlineStr">
         <is>
-          <t>21/10/2023 15:24</t>
+          <t>21/10/2023 15:29</t>
         </is>
       </c>
       <c r="N69" t="n">
-        <v>4.28</v>
+        <v>5.15</v>
       </c>
       <c r="O69" t="inlineStr">
         <is>
-          <t>01/10/2023 23:02</t>
+          <t>02/10/2023 08:32</t>
         </is>
       </c>
       <c r="P69" t="n">
-        <v>3.91</v>
+        <v>5.1</v>
       </c>
       <c r="Q69" t="inlineStr">
         <is>
-          <t>21/10/2023 15:27</t>
+          <t>21/10/2023 15:29</t>
         </is>
       </c>
       <c r="R69" t="n">
-        <v>5.28</v>
+        <v>1.4</v>
       </c>
       <c r="S69" t="inlineStr">
         <is>
-          <t>01/10/2023 23:02</t>
+          <t>02/10/2023 08:32</t>
         </is>
       </c>
       <c r="T69" t="n">
-        <v>4.61</v>
+        <v>1.47</v>
       </c>
       <c r="U69" t="inlineStr">
         <is>
-          <t>21/10/2023 15:26</t>
+          <t>21/10/2023 15:28</t>
         </is>
       </c>
       <c r="V69" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/freiburg-bochum/rZG64nQN/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/darmstadt-rb-leipzig/2wlXK7A4/</t>
         </is>
       </c>
     </row>
@@ -6829,71 +6829,71 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Darmstadt</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G70" t="n">
+        <v>2</v>
+      </c>
+      <c r="H70" t="inlineStr">
+        <is>
+          <t>Bochum</t>
+        </is>
+      </c>
+      <c r="I70" t="n">
         <v>1</v>
       </c>
-      <c r="H70" t="inlineStr">
-        <is>
-          <t>RB Leipzig</t>
-        </is>
-      </c>
-      <c r="I70" t="n">
-        <v>3</v>
-      </c>
       <c r="J70" t="n">
-        <v>6.5</v>
+        <v>1.56</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
-          <t>02/10/2023 08:32</t>
+          <t>01/10/2023 23:02</t>
         </is>
       </c>
       <c r="L70" t="n">
-        <v>6.59</v>
+        <v>1.81</v>
       </c>
       <c r="M70" t="inlineStr">
         <is>
-          <t>21/10/2023 15:29</t>
+          <t>21/10/2023 15:24</t>
         </is>
       </c>
       <c r="N70" t="n">
-        <v>5.15</v>
+        <v>4.28</v>
       </c>
       <c r="O70" t="inlineStr">
         <is>
-          <t>02/10/2023 08:32</t>
+          <t>01/10/2023 23:02</t>
         </is>
       </c>
       <c r="P70" t="n">
-        <v>5.1</v>
+        <v>3.91</v>
       </c>
       <c r="Q70" t="inlineStr">
         <is>
-          <t>21/10/2023 15:29</t>
+          <t>21/10/2023 15:27</t>
         </is>
       </c>
       <c r="R70" t="n">
-        <v>1.4</v>
+        <v>5.28</v>
       </c>
       <c r="S70" t="inlineStr">
         <is>
-          <t>02/10/2023 08:32</t>
+          <t>01/10/2023 23:02</t>
         </is>
       </c>
       <c r="T70" t="n">
-        <v>1.47</v>
+        <v>4.61</v>
       </c>
       <c r="U70" t="inlineStr">
         <is>
-          <t>21/10/2023 15:28</t>
+          <t>21/10/2023 15:26</t>
         </is>
       </c>
       <c r="V70" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/darmstadt-rb-leipzig/2wlXK7A4/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/freiburg-bochum/rZG64nQN/</t>
         </is>
       </c>
     </row>
@@ -9773,7 +9773,7 @@
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="G102" t="n">
@@ -9781,14 +9781,14 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>Darmstadt</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="I102" t="n">
         <v>1</v>
       </c>
       <c r="J102" t="n">
-        <v>1.53</v>
+        <v>1.65</v>
       </c>
       <c r="K102" t="inlineStr">
         <is>
@@ -9796,7 +9796,7 @@
         </is>
       </c>
       <c r="L102" t="n">
-        <v>1.53</v>
+        <v>1.99</v>
       </c>
       <c r="M102" t="inlineStr">
         <is>
@@ -9804,7 +9804,7 @@
         </is>
       </c>
       <c r="N102" t="n">
-        <v>4.43</v>
+        <v>3.96</v>
       </c>
       <c r="O102" t="inlineStr">
         <is>
@@ -9812,32 +9812,32 @@
         </is>
       </c>
       <c r="P102" t="n">
-        <v>4.55</v>
+        <v>3.59</v>
       </c>
       <c r="Q102" t="inlineStr">
         <is>
+          <t>25/11/2023 15:27</t>
+        </is>
+      </c>
+      <c r="R102" t="n">
+        <v>5.46</v>
+      </c>
+      <c r="S102" t="inlineStr">
+        <is>
+          <t>05/11/2023 11:03</t>
+        </is>
+      </c>
+      <c r="T102" t="n">
+        <v>4.02</v>
+      </c>
+      <c r="U102" t="inlineStr">
+        <is>
           <t>25/11/2023 15:28</t>
         </is>
       </c>
-      <c r="R102" t="n">
-        <v>6.12</v>
-      </c>
-      <c r="S102" t="inlineStr">
-        <is>
-          <t>05/11/2023 11:03</t>
-        </is>
-      </c>
-      <c r="T102" t="n">
-        <v>6.28</v>
-      </c>
-      <c r="U102" t="inlineStr">
-        <is>
-          <t>25/11/2023 15:28</t>
-        </is>
-      </c>
       <c r="V102" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/freiburg-darmstadt/OlSgQN3s/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/union-berlin-augsburg/ldySU3eQ/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Dortmund</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Bayer Leverkusen</t>
+          <t>B. Monchengladbach</t>
         </is>
       </c>
       <c r="I104" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J104" t="n">
-        <v>5.02</v>
+        <v>1.35</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,15 +9980,15 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>6</v>
+        <v>1.51</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>25/11/2023 15:26</t>
+          <t>25/11/2023 14:49</t>
         </is>
       </c>
       <c r="N104" t="n">
-        <v>4.42</v>
+        <v>5.88</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>5.11</v>
+        <v>5.24</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>25/11/2023 15:26</t>
+          <t>25/11/2023 15:27</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>1.62</v>
+        <v>7.58</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,16 +10012,16 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>1.47</v>
+        <v>5.53</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>25/11/2023 13:02</t>
+          <t>25/11/2023 15:28</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/werder-bremen-bayer-leverkusen/niJELaIC/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/dortmund-b-monchengladbach/6XoNVqtK/</t>
         </is>
       </c>
     </row>
@@ -10049,22 +10049,22 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Dortmund</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>B. Monchengladbach</t>
+          <t>Darmstadt</t>
         </is>
       </c>
       <c r="I105" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J105" t="n">
-        <v>1.35</v>
+        <v>1.53</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -10072,15 +10072,15 @@
         </is>
       </c>
       <c r="L105" t="n">
-        <v>1.51</v>
+        <v>1.53</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>25/11/2023 14:49</t>
+          <t>25/11/2023 15:28</t>
         </is>
       </c>
       <c r="N105" t="n">
-        <v>5.88</v>
+        <v>4.43</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -10088,15 +10088,15 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>5.24</v>
+        <v>4.55</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>25/11/2023 15:27</t>
+          <t>25/11/2023 15:28</t>
         </is>
       </c>
       <c r="R105" t="n">
-        <v>7.58</v>
+        <v>6.12</v>
       </c>
       <c r="S105" t="inlineStr">
         <is>
@@ -10104,7 +10104,7 @@
         </is>
       </c>
       <c r="T105" t="n">
-        <v>5.53</v>
+        <v>6.28</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
@@ -10113,7 +10113,7 @@
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/dortmund-b-monchengladbach/6XoNVqtK/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/freiburg-darmstadt/OlSgQN3s/</t>
         </is>
       </c>
     </row>
@@ -10141,22 +10141,22 @@
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H106" t="inlineStr">
         <is>
-          <t>Augsburg</t>
+          <t>Bayer Leverkusen</t>
         </is>
       </c>
       <c r="I106" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J106" t="n">
-        <v>1.65</v>
+        <v>5.02</v>
       </c>
       <c r="K106" t="inlineStr">
         <is>
@@ -10164,15 +10164,15 @@
         </is>
       </c>
       <c r="L106" t="n">
-        <v>1.99</v>
+        <v>6</v>
       </c>
       <c r="M106" t="inlineStr">
         <is>
-          <t>25/11/2023 15:28</t>
+          <t>25/11/2023 15:26</t>
         </is>
       </c>
       <c r="N106" t="n">
-        <v>3.96</v>
+        <v>4.42</v>
       </c>
       <c r="O106" t="inlineStr">
         <is>
@@ -10180,15 +10180,15 @@
         </is>
       </c>
       <c r="P106" t="n">
-        <v>3.59</v>
+        <v>5.11</v>
       </c>
       <c r="Q106" t="inlineStr">
         <is>
-          <t>25/11/2023 15:27</t>
+          <t>25/11/2023 15:26</t>
         </is>
       </c>
       <c r="R106" t="n">
-        <v>5.46</v>
+        <v>1.62</v>
       </c>
       <c r="S106" t="inlineStr">
         <is>
@@ -10196,16 +10196,16 @@
         </is>
       </c>
       <c r="T106" t="n">
-        <v>4.02</v>
+        <v>1.47</v>
       </c>
       <c r="U106" t="inlineStr">
         <is>
-          <t>25/11/2023 15:28</t>
+          <t>25/11/2023 13:02</t>
         </is>
       </c>
       <c r="V106" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/union-berlin-augsburg/ldySU3eQ/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/werder-bremen-bayer-leverkusen/niJELaIC/</t>
         </is>
       </c>
     </row>
@@ -11337,22 +11337,22 @@
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Werder Bremen</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H119" t="inlineStr">
         <is>
-          <t>B. Monchengladbach</t>
+          <t>Augsburg</t>
         </is>
       </c>
       <c r="I119" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J119" t="n">
-        <v>1.75</v>
+        <v>1.93</v>
       </c>
       <c r="K119" t="inlineStr">
         <is>
@@ -11360,15 +11360,15 @@
         </is>
       </c>
       <c r="L119" t="n">
-        <v>2.09</v>
+        <v>2.21</v>
       </c>
       <c r="M119" t="inlineStr">
         <is>
-          <t>09/12/2023 15:28</t>
+          <t>09/12/2023 15:29</t>
         </is>
       </c>
       <c r="N119" t="n">
-        <v>3.86</v>
+        <v>3.83</v>
       </c>
       <c r="O119" t="inlineStr">
         <is>
@@ -11376,15 +11376,15 @@
         </is>
       </c>
       <c r="P119" t="n">
-        <v>3.54</v>
+        <v>3.73</v>
       </c>
       <c r="Q119" t="inlineStr">
         <is>
-          <t>09/12/2023 15:28</t>
+          <t>09/12/2023 15:29</t>
         </is>
       </c>
       <c r="R119" t="n">
-        <v>4.25</v>
+        <v>3.5</v>
       </c>
       <c r="S119" t="inlineStr">
         <is>
@@ -11392,16 +11392,16 @@
         </is>
       </c>
       <c r="T119" t="n">
-        <v>3.74</v>
+        <v>3.25</v>
       </c>
       <c r="U119" t="inlineStr">
         <is>
-          <t>09/12/2023 15:28</t>
+          <t>09/12/2023 15:29</t>
         </is>
       </c>
       <c r="V119" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/union-berlin-b-monchengladbach/S8q8uf9o/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/werder-bremen-augsburg/fZgSzWNG/</t>
         </is>
       </c>
     </row>
@@ -11429,22 +11429,22 @@
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Union Berlin</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H120" t="inlineStr">
         <is>
-          <t>Freiburg</t>
+          <t>B. Monchengladbach</t>
         </is>
       </c>
       <c r="I120" t="n">
         <v>1</v>
       </c>
       <c r="J120" t="n">
-        <v>1.95</v>
+        <v>1.75</v>
       </c>
       <c r="K120" t="inlineStr">
         <is>
@@ -11452,15 +11452,15 @@
         </is>
       </c>
       <c r="L120" t="n">
-        <v>2.22</v>
+        <v>2.09</v>
       </c>
       <c r="M120" t="inlineStr">
         <is>
-          <t>09/12/2023 15:29</t>
+          <t>09/12/2023 15:28</t>
         </is>
       </c>
       <c r="N120" t="n">
-        <v>3.84</v>
+        <v>3.86</v>
       </c>
       <c r="O120" t="inlineStr">
         <is>
@@ -11472,11 +11472,11 @@
       </c>
       <c r="Q120" t="inlineStr">
         <is>
-          <t>09/12/2023 15:29</t>
+          <t>09/12/2023 15:28</t>
         </is>
       </c>
       <c r="R120" t="n">
-        <v>3.45</v>
+        <v>4.25</v>
       </c>
       <c r="S120" t="inlineStr">
         <is>
@@ -11484,16 +11484,16 @@
         </is>
       </c>
       <c r="T120" t="n">
-        <v>3.39</v>
+        <v>3.74</v>
       </c>
       <c r="U120" t="inlineStr">
         <is>
-          <t>09/12/2023 15:29</t>
+          <t>09/12/2023 15:28</t>
         </is>
       </c>
       <c r="V120" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/wolfsburg-freiburg/8IiGwYwb/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/union-berlin-b-monchengladbach/S8q8uf9o/</t>
         </is>
       </c>
     </row>
@@ -11521,22 +11521,22 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Eintracht Frankfurt</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="H121" t="inlineStr">
         <is>
-          <t>Bayern Munich</t>
+          <t>Freiburg</t>
         </is>
       </c>
       <c r="I121" t="n">
         <v>1</v>
       </c>
       <c r="J121" t="n">
-        <v>5.86</v>
+        <v>1.95</v>
       </c>
       <c r="K121" t="inlineStr">
         <is>
@@ -11544,7 +11544,7 @@
         </is>
       </c>
       <c r="L121" t="n">
-        <v>8.949999999999999</v>
+        <v>2.22</v>
       </c>
       <c r="M121" t="inlineStr">
         <is>
@@ -11552,7 +11552,7 @@
         </is>
       </c>
       <c r="N121" t="n">
-        <v>5.08</v>
+        <v>3.84</v>
       </c>
       <c r="O121" t="inlineStr">
         <is>
@@ -11560,7 +11560,7 @@
         </is>
       </c>
       <c r="P121" t="n">
-        <v>6.12</v>
+        <v>3.54</v>
       </c>
       <c r="Q121" t="inlineStr">
         <is>
@@ -11568,7 +11568,7 @@
         </is>
       </c>
       <c r="R121" t="n">
-        <v>1.48</v>
+        <v>3.45</v>
       </c>
       <c r="S121" t="inlineStr">
         <is>
@@ -11576,16 +11576,16 @@
         </is>
       </c>
       <c r="T121" t="n">
-        <v>1.32</v>
+        <v>3.39</v>
       </c>
       <c r="U121" t="inlineStr">
         <is>
-          <t>09/12/2023 15:27</t>
+          <t>09/12/2023 15:29</t>
         </is>
       </c>
       <c r="V121" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/eintracht-frankfurt-bayern-munich/Qg2BvEOi/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/wolfsburg-freiburg/8IiGwYwb/</t>
         </is>
       </c>
     </row>
@@ -11613,22 +11613,22 @@
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Heidenheim</t>
+          <t>Eintracht Frankfurt</t>
         </is>
       </c>
       <c r="G122" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H122" t="inlineStr">
         <is>
-          <t>Darmstadt</t>
+          <t>Bayern Munich</t>
         </is>
       </c>
       <c r="I122" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J122" t="n">
-        <v>1.99</v>
+        <v>5.86</v>
       </c>
       <c r="K122" t="inlineStr">
         <is>
@@ -11636,48 +11636,48 @@
         </is>
       </c>
       <c r="L122" t="n">
-        <v>1.82</v>
+        <v>8.949999999999999</v>
       </c>
       <c r="M122" t="inlineStr">
         <is>
+          <t>09/12/2023 15:29</t>
+        </is>
+      </c>
+      <c r="N122" t="n">
+        <v>5.08</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>25/11/2023 22:02</t>
+        </is>
+      </c>
+      <c r="P122" t="n">
+        <v>6.12</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>09/12/2023 15:29</t>
+        </is>
+      </c>
+      <c r="R122" t="n">
+        <v>1.48</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>25/11/2023 22:02</t>
+        </is>
+      </c>
+      <c r="T122" t="n">
+        <v>1.32</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
           <t>09/12/2023 15:27</t>
         </is>
       </c>
-      <c r="N122" t="n">
-        <v>3.83</v>
-      </c>
-      <c r="O122" t="inlineStr">
-        <is>
-          <t>25/11/2023 22:02</t>
-        </is>
-      </c>
-      <c r="P122" t="n">
-        <v>3.96</v>
-      </c>
-      <c r="Q122" t="inlineStr">
-        <is>
-          <t>09/12/2023 15:28</t>
-        </is>
-      </c>
-      <c r="R122" t="n">
-        <v>3.36</v>
-      </c>
-      <c r="S122" t="inlineStr">
-        <is>
-          <t>25/11/2023 22:02</t>
-        </is>
-      </c>
-      <c r="T122" t="n">
-        <v>4.4</v>
-      </c>
-      <c r="U122" t="inlineStr">
-        <is>
-          <t>09/12/2023 15:28</t>
-        </is>
-      </c>
       <c r="V122" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/heidenheim-darmstadt/j1myZ9hT/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/eintracht-frankfurt-bayern-munich/Qg2BvEOi/</t>
         </is>
       </c>
     </row>
@@ -11705,22 +11705,22 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Werder Bremen</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="G123" t="n">
+        <v>3</v>
+      </c>
+      <c r="H123" t="inlineStr">
+        <is>
+          <t>Darmstadt</t>
+        </is>
+      </c>
+      <c r="I123" t="n">
         <v>2</v>
       </c>
-      <c r="H123" t="inlineStr">
-        <is>
-          <t>Augsburg</t>
-        </is>
-      </c>
-      <c r="I123" t="n">
-        <v>0</v>
-      </c>
       <c r="J123" t="n">
-        <v>1.93</v>
+        <v>1.99</v>
       </c>
       <c r="K123" t="inlineStr">
         <is>
@@ -11728,11 +11728,11 @@
         </is>
       </c>
       <c r="L123" t="n">
-        <v>2.21</v>
+        <v>1.82</v>
       </c>
       <c r="M123" t="inlineStr">
         <is>
-          <t>09/12/2023 15:29</t>
+          <t>09/12/2023 15:27</t>
         </is>
       </c>
       <c r="N123" t="n">
@@ -11744,15 +11744,15 @@
         </is>
       </c>
       <c r="P123" t="n">
-        <v>3.73</v>
+        <v>3.96</v>
       </c>
       <c r="Q123" t="inlineStr">
         <is>
-          <t>09/12/2023 15:29</t>
+          <t>09/12/2023 15:28</t>
         </is>
       </c>
       <c r="R123" t="n">
-        <v>3.5</v>
+        <v>3.36</v>
       </c>
       <c r="S123" t="inlineStr">
         <is>
@@ -11760,16 +11760,16 @@
         </is>
       </c>
       <c r="T123" t="n">
-        <v>3.25</v>
+        <v>4.4</v>
       </c>
       <c r="U123" t="inlineStr">
         <is>
-          <t>09/12/2023 15:29</t>
+          <t>09/12/2023 15:28</t>
         </is>
       </c>
       <c r="V123" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/werder-bremen-augsburg/fZgSzWNG/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/heidenheim-darmstadt/j1myZ9hT/</t>
         </is>
       </c>
     </row>
@@ -12165,7 +12165,7 @@
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Darmstadt</t>
+          <t>Mainz</t>
         </is>
       </c>
       <c r="G128" t="n">
@@ -12173,14 +12173,14 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>Wolfsburg</t>
+          <t>Heidenheim</t>
         </is>
       </c>
       <c r="I128" t="n">
         <v>1</v>
       </c>
       <c r="J128" t="n">
-        <v>3.05</v>
+        <v>1.65</v>
       </c>
       <c r="K128" t="inlineStr">
         <is>
@@ -12188,15 +12188,15 @@
         </is>
       </c>
       <c r="L128" t="n">
-        <v>3.97</v>
+        <v>1.72</v>
       </c>
       <c r="M128" t="inlineStr">
         <is>
-          <t>16/12/2023 15:26</t>
+          <t>16/12/2023 15:29</t>
         </is>
       </c>
       <c r="N128" t="n">
-        <v>3.58</v>
+        <v>4.07</v>
       </c>
       <c r="O128" t="inlineStr">
         <is>
@@ -12204,15 +12204,15 @@
         </is>
       </c>
       <c r="P128" t="n">
-        <v>3.86</v>
+        <v>4.14</v>
       </c>
       <c r="Q128" t="inlineStr">
         <is>
-          <t>16/12/2023 15:26</t>
+          <t>16/12/2023 15:29</t>
         </is>
       </c>
       <c r="R128" t="n">
-        <v>2.19</v>
+        <v>4.58</v>
       </c>
       <c r="S128" t="inlineStr">
         <is>
@@ -12220,16 +12220,16 @@
         </is>
       </c>
       <c r="T128" t="n">
-        <v>1.93</v>
+        <v>4.82</v>
       </c>
       <c r="U128" t="inlineStr">
         <is>
-          <t>16/12/2023 15:26</t>
+          <t>16/12/2023 15:29</t>
         </is>
       </c>
       <c r="V128" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/darmstadt-wolfsburg/OUZ6nTMS/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/mainz-heidenheim/KxwjjBN3/</t>
         </is>
       </c>
     </row>
@@ -12257,22 +12257,22 @@
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Bochum</t>
+          <t>Darmstadt</t>
         </is>
       </c>
       <c r="G129" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="H129" t="inlineStr">
         <is>
-          <t>Union Berlin</t>
+          <t>Wolfsburg</t>
         </is>
       </c>
       <c r="I129" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J129" t="n">
-        <v>2.65</v>
+        <v>3.05</v>
       </c>
       <c r="K129" t="inlineStr">
         <is>
@@ -12280,15 +12280,15 @@
         </is>
       </c>
       <c r="L129" t="n">
-        <v>2.62</v>
+        <v>3.97</v>
       </c>
       <c r="M129" t="inlineStr">
         <is>
-          <t>16/12/2023 15:29</t>
+          <t>16/12/2023 15:26</t>
         </is>
       </c>
       <c r="N129" t="n">
-        <v>3.25</v>
+        <v>3.58</v>
       </c>
       <c r="O129" t="inlineStr">
         <is>
@@ -12296,15 +12296,15 @@
         </is>
       </c>
       <c r="P129" t="n">
-        <v>3.36</v>
+        <v>3.86</v>
       </c>
       <c r="Q129" t="inlineStr">
         <is>
-          <t>16/12/2023 15:29</t>
+          <t>16/12/2023 15:26</t>
         </is>
       </c>
       <c r="R129" t="n">
-        <v>2.63</v>
+        <v>2.19</v>
       </c>
       <c r="S129" t="inlineStr">
         <is>
@@ -12312,16 +12312,16 @@
         </is>
       </c>
       <c r="T129" t="n">
-        <v>2.88</v>
+        <v>1.93</v>
       </c>
       <c r="U129" t="inlineStr">
         <is>
-          <t>16/12/2023 15:29</t>
+          <t>16/12/2023 15:26</t>
         </is>
       </c>
       <c r="V129" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/bochum-union-berlin/G4WblkhG/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/darmstadt-wolfsburg/OUZ6nTMS/</t>
         </is>
       </c>
     </row>
@@ -12441,22 +12441,22 @@
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Mainz</t>
+          <t>Bochum</t>
         </is>
       </c>
       <c r="G131" t="n">
+        <v>3</v>
+      </c>
+      <c r="H131" t="inlineStr">
+        <is>
+          <t>Union Berlin</t>
+        </is>
+      </c>
+      <c r="I131" t="n">
         <v>0</v>
       </c>
-      <c r="H131" t="inlineStr">
-        <is>
-          <t>Heidenheim</t>
-        </is>
-      </c>
-      <c r="I131" t="n">
-        <v>1</v>
-      </c>
       <c r="J131" t="n">
-        <v>1.65</v>
+        <v>2.65</v>
       </c>
       <c r="K131" t="inlineStr">
         <is>
@@ -12464,7 +12464,7 @@
         </is>
       </c>
       <c r="L131" t="n">
-        <v>1.72</v>
+        <v>2.62</v>
       </c>
       <c r="M131" t="inlineStr">
         <is>
@@ -12472,7 +12472,7 @@
         </is>
       </c>
       <c r="N131" t="n">
-        <v>4.07</v>
+        <v>3.25</v>
       </c>
       <c r="O131" t="inlineStr">
         <is>
@@ -12480,7 +12480,7 @@
         </is>
       </c>
       <c r="P131" t="n">
-        <v>4.14</v>
+        <v>3.36</v>
       </c>
       <c r="Q131" t="inlineStr">
         <is>
@@ -12488,7 +12488,7 @@
         </is>
       </c>
       <c r="R131" t="n">
-        <v>4.58</v>
+        <v>2.63</v>
       </c>
       <c r="S131" t="inlineStr">
         <is>
@@ -12496,7 +12496,7 @@
         </is>
       </c>
       <c r="T131" t="n">
-        <v>4.82</v>
+        <v>2.88</v>
       </c>
       <c r="U131" t="inlineStr">
         <is>
@@ -12505,7 +12505,7 @@
       </c>
       <c r="V131" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/germany/bundesliga/mainz-heidenheim/KxwjjBN3/</t>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/bochum-union-berlin/G4WblkhG/</t>
         </is>
       </c>
     </row>
@@ -12874,6 +12874,282 @@
       <c r="V135" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/germany/bundesliga/bayern-munich-vfb-stuttgart/8tz3UT0p/</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" s="1" t="n">
+        <v>135</v>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>germany</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>bundesliga</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E136" s="2" t="n">
+        <v>45279.77083333334</v>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Werder Bremen</t>
+        </is>
+      </c>
+      <c r="G136" t="n">
+        <v>1</v>
+      </c>
+      <c r="H136" t="inlineStr">
+        <is>
+          <t>RB Leipzig</t>
+        </is>
+      </c>
+      <c r="I136" t="n">
+        <v>1</v>
+      </c>
+      <c r="J136" t="n">
+        <v>4.03</v>
+      </c>
+      <c r="K136" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="L136" t="n">
+        <v>5.56</v>
+      </c>
+      <c r="M136" t="inlineStr">
+        <is>
+          <t>19/12/2023 18:28</t>
+        </is>
+      </c>
+      <c r="N136" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="O136" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="P136" t="n">
+        <v>4.71</v>
+      </c>
+      <c r="Q136" t="inlineStr">
+        <is>
+          <t>19/12/2023 18:28</t>
+        </is>
+      </c>
+      <c r="R136" t="n">
+        <v>1.71</v>
+      </c>
+      <c r="S136" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="T136" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="U136" t="inlineStr">
+        <is>
+          <t>19/12/2023 18:25</t>
+        </is>
+      </c>
+      <c r="V136" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/werder-bremen-rb-leipzig/8bex28MF/</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" s="1" t="n">
+        <v>136</v>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>germany</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>bundesliga</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E137" s="2" t="n">
+        <v>45279.85416666666</v>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Hoffenheim</t>
+        </is>
+      </c>
+      <c r="G137" t="n">
+        <v>3</v>
+      </c>
+      <c r="H137" t="inlineStr">
+        <is>
+          <t>Darmstadt</t>
+        </is>
+      </c>
+      <c r="I137" t="n">
+        <v>3</v>
+      </c>
+      <c r="J137" t="n">
+        <v>1.54</v>
+      </c>
+      <c r="K137" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="L137" t="n">
+        <v>1.51</v>
+      </c>
+      <c r="M137" t="inlineStr">
+        <is>
+          <t>19/12/2023 20:02</t>
+        </is>
+      </c>
+      <c r="N137" t="n">
+        <v>4.46</v>
+      </c>
+      <c r="O137" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="P137" t="n">
+        <v>4.74</v>
+      </c>
+      <c r="Q137" t="inlineStr">
+        <is>
+          <t>19/12/2023 20:28</t>
+        </is>
+      </c>
+      <c r="R137" t="n">
+        <v>4.99</v>
+      </c>
+      <c r="S137" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="T137" t="n">
+        <v>6.42</v>
+      </c>
+      <c r="U137" t="inlineStr">
+        <is>
+          <t>19/12/2023 20:28</t>
+        </is>
+      </c>
+      <c r="V137" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/hoffenheim-darmstadt/U7dY2l79/</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" s="1" t="n">
+        <v>137</v>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>germany</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>bundesliga</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E138" s="2" t="n">
+        <v>45279.85416666666</v>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Dortmund</t>
+        </is>
+      </c>
+      <c r="G138" t="n">
+        <v>1</v>
+      </c>
+      <c r="H138" t="inlineStr">
+        <is>
+          <t>Mainz</t>
+        </is>
+      </c>
+      <c r="I138" t="n">
+        <v>1</v>
+      </c>
+      <c r="J138" t="n">
+        <v>1.34</v>
+      </c>
+      <c r="K138" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="L138" t="n">
+        <v>1.56</v>
+      </c>
+      <c r="M138" t="inlineStr">
+        <is>
+          <t>19/12/2023 20:08</t>
+        </is>
+      </c>
+      <c r="N138" t="n">
+        <v>5.47</v>
+      </c>
+      <c r="O138" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="P138" t="n">
+        <v>4.63</v>
+      </c>
+      <c r="Q138" t="inlineStr">
+        <is>
+          <t>19/12/2023 20:08</t>
+        </is>
+      </c>
+      <c r="R138" t="n">
+        <v>6.8</v>
+      </c>
+      <c r="S138" t="inlineStr">
+        <is>
+          <t>09/12/2023 20:03</t>
+        </is>
+      </c>
+      <c r="T138" t="n">
+        <v>5.73</v>
+      </c>
+      <c r="U138" t="inlineStr">
+        <is>
+          <t>19/12/2023 20:08</t>
+        </is>
+      </c>
+      <c r="V138" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/germany/bundesliga/dortmund-mainz/QwMYsmVq/</t>
         </is>
       </c>
     </row>

</xml_diff>